<commit_message>
built out functionality of flux mapping
</commit_message>
<xml_diff>
--- a/data/13c_mfa/INCA_model_11022023_GR.xlsx
+++ b/data/13c_mfa/INCA_model_11022023_GR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrettroell/yarrowia_eflux2/data/13c_mfa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8936FD2-6D49-014A-93BE-BC03E59BAA26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E4CD8C-69B5-D842-83F2-60D1C66DB60F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="18900" firstSheet="1" activeTab="3" xr2:uid="{2683B27E-BA21-2341-8B90-63D55B06C26E}"/>
+    <workbookView xWindow="280" yWindow="3800" windowWidth="35840" windowHeight="18900" firstSheet="1" activeTab="3" xr2:uid="{2683B27E-BA21-2341-8B90-63D55B06C26E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1923" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1910" uniqueCount="286">
   <si>
     <t>ID</t>
   </si>
@@ -765,33 +765,9 @@
     <t>YL_10232023_glyc</t>
   </si>
   <si>
-    <t>YL_11022023_gluc</t>
-  </si>
-  <si>
-    <t>YL_11022023_glyc</t>
-  </si>
-  <si>
-    <t>YL_11022023_OA</t>
-  </si>
-  <si>
     <t>R80</t>
   </si>
   <si>
-    <t>biomass glucose</t>
-  </si>
-  <si>
-    <t>biomass glycerol</t>
-  </si>
-  <si>
-    <t>biomass oleic acid</t>
-  </si>
-  <si>
-    <t>0.38*ALA + 0.13*ARG + 0.165*ASN + 0.165*ASP + 0.0036*CYS + 0.26*GLN + 0.26*GLU + 0.29*GLY + 0.06*HIS + 0.15*ILE + 0.24*LEU + 0.24*LYS + 0.0442*MET + 0.13*PHE + 0.15*PRO + 0.22*SER + 0.2105*THR + 0.0022*TRP + 0.06*TYR + 0.2*VAL + 3.902*ACCOAcyt + 0.186*DHAP + 3.902*ATP + 7.804*NADPH + 0.186*NADH + 0.123*R5P + 0.152*ASP + 0.06*GLY + 1.7*G6P -&gt; biomass + 0.076*FUM</t>
-  </si>
-  <si>
-    <t>0.19*ALA + 0.08*ARG + 0.09*ASN + 0.09*ASP + 0.0036*CYS + 0.145*GLN + 0.145*GLU + 0.17*GLY + 0.03*HIS + 0.09*ILE + 0.14*LEU + 0.06*LYS + 0.0442*MET + 0.08*PHE + 0.12*PRO + 0.11*SER + 0.2105*THR + 0.0022*TRP + 0.05*TYR + 0.13*VAL + 6.503*ACCOAcyt + 0.31*DHAP + 6.503*ATP + 13.01*NADPH + 0.31*NADH + 0.123*R5P + 0.152*ASP + 0.06*GLY + 1.7*G6P -&gt; biomass + 0.076*FUM</t>
-  </si>
-  <si>
     <t>Location on map</t>
   </si>
   <si>
@@ -810,9 +786,6 @@
     <t>(-1184, 515)</t>
   </si>
   <si>
-    <t>(-984, 290)</t>
-  </si>
-  <si>
     <t>(-700, 250)</t>
   </si>
   <si>
@@ -849,18 +822,12 @@
     <t>(-324, 1175)</t>
   </si>
   <si>
-    <t>(400, -226)</t>
-  </si>
-  <si>
     <t>(818, -383)</t>
   </si>
   <si>
     <t>(980, -618)</t>
   </si>
   <si>
-    <t>(1176, -797)</t>
-  </si>
-  <si>
     <t>(971, -1014)</t>
   </si>
   <si>
@@ -910,6 +877,27 @@
   </si>
   <si>
     <t>(-55, 111)</t>
+  </si>
+  <si>
+    <t>(1154, -746)</t>
+  </si>
+  <si>
+    <t>(1154, -825)</t>
+  </si>
+  <si>
+    <t>(-984, 273)</t>
+  </si>
+  <si>
+    <t>(320, -226)</t>
+  </si>
+  <si>
+    <t>biomass_C or biomass_glucose or biomass_oil</t>
+  </si>
+  <si>
+    <t>(-1670, -1049)</t>
+  </si>
+  <si>
+    <t>(-1670, -1155)</t>
   </si>
 </sst>
 </file>
@@ -15678,8 +15666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFD0AB96-9F04-41BF-A187-22CBB81F1551}">
   <dimension ref="A1:V86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15710,7 +15698,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
@@ -15778,7 +15766,7 @@
         <v>24</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="H2" s="3">
         <v>100</v>
@@ -15824,7 +15812,7 @@
         <v>24</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="4"/>
@@ -15911,7 +15899,7 @@
         <v>24</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="H5" s="11"/>
       <c r="I5" s="12"/>
@@ -15957,7 +15945,7 @@
         <v>24</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="H6" s="17">
         <v>19.0701</v>
@@ -16025,7 +16013,7 @@
         <v>24</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="H7" s="17">
         <v>58.152200000000001</v>
@@ -16093,7 +16081,7 @@
         <v>24</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H8" s="17">
         <v>58.152200000000001</v>
@@ -16161,7 +16149,7 @@
         <v>24</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>256</v>
+        <v>281</v>
       </c>
       <c r="H9" s="17">
         <v>56.058100000000003</v>
@@ -16229,7 +16217,7 @@
         <v>24</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="H10" s="17">
         <v>132.6942</v>
@@ -16297,7 +16285,7 @@
         <v>24</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="H11" s="17">
         <v>128.75890000000001</v>
@@ -16365,7 +16353,7 @@
         <v>24</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="H12" s="17">
         <v>126.63800000000001</v>
@@ -16433,7 +16421,7 @@
         <v>24</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="H13" s="18">
         <v>2.2069000000000001</v>
@@ -16501,7 +16489,7 @@
         <v>24</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="H14" s="17">
         <v>61.790199999999999</v>
@@ -16569,7 +16557,7 @@
         <v>24</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="H15" s="17">
         <v>61.790199999999999</v>
@@ -16637,7 +16625,7 @@
         <v>24</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="H16" s="17">
         <v>22.708100000000002</v>
@@ -16705,7 +16693,7 @@
         <v>24</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="H17" s="17">
         <v>39.082099999999997</v>
@@ -16773,7 +16761,7 @@
         <v>24</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="H18" s="17">
         <v>39.082099999999997</v>
@@ -16841,7 +16829,7 @@
         <v>24</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="H19" s="17">
         <v>18.459099999999999</v>
@@ -16909,7 +16897,7 @@
         <v>24</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="H20" s="17">
         <v>20.623000000000001</v>
@@ -16977,7 +16965,7 @@
         <v>24</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="H21" s="17">
         <v>20.623000000000001</v>
@@ -17045,7 +17033,7 @@
         <v>24</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="H22" s="18">
         <v>20.623000000000001</v>
@@ -17113,7 +17101,7 @@
         <v>94</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>269</v>
+        <v>282</v>
       </c>
       <c r="H23" s="17">
         <v>97.212199999999996</v>
@@ -17181,7 +17169,7 @@
         <v>94</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="H24" s="17">
         <v>37.553899999999999</v>
@@ -17249,7 +17237,7 @@
         <v>94</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="H25" s="17">
         <v>24.903500000000001</v>
@@ -17317,7 +17305,7 @@
         <v>94</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="H26" s="17">
         <v>24.903500000000001</v>
@@ -17385,7 +17373,7 @@
         <v>94</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="H27" s="17">
         <v>1.0003E-7</v>
@@ -17453,7 +17441,7 @@
         <v>94</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="H28" s="17">
         <v>13.1945</v>
@@ -17521,7 +17509,7 @@
         <v>94</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="H29" s="17">
         <v>25.844899999999999</v>
@@ -17589,7 +17577,7 @@
         <v>94</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="H30" s="17">
         <v>27.984100000000002</v>
@@ -17657,7 +17645,7 @@
         <v>94</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="H31" s="18">
         <v>37.553899999999999</v>
@@ -17725,7 +17713,7 @@
         <v>94</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="H32" s="17">
         <v>-9.5698000000000008</v>
@@ -17793,7 +17781,7 @@
         <v>24</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="H33" s="17">
         <v>4.0061</v>
@@ -18047,7 +18035,7 @@
         <v>137</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="H37" s="17">
         <v>12.650399999999999</v>
@@ -18115,7 +18103,7 @@
         <v>24</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="H38" s="17">
         <v>12.650399999999999</v>
@@ -18183,7 +18171,7 @@
         <v>24</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="H39" s="17">
         <v>12.650399999999999</v>
@@ -18251,7 +18239,7 @@
         <v>24</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="H40" s="18">
         <v>12.650399999999999</v>
@@ -18319,7 +18307,7 @@
         <v>94</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="H41" s="17">
         <v>122.6567</v>
@@ -18378,7 +18366,7 @@
         <v>154</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="H42" s="17">
         <v>-56.956200000000003</v>
@@ -18446,7 +18434,7 @@
         <v>94</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="H43" s="17">
         <v>12.650399999999999</v>
@@ -18514,7 +18502,7 @@
         <v>94</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="H44" s="17">
         <v>12.650399999999999</v>
@@ -18582,7 +18570,7 @@
         <v>94</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="H45" s="18">
         <v>0</v>
@@ -19889,10 +19877,10 @@
         <v>209</v>
       </c>
       <c r="B68" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D68" t="s">
-        <v>212</v>
+        <v>283</v>
       </c>
       <c r="E68" t="s">
         <v>213</v>
@@ -19900,7 +19888,9 @@
       <c r="F68" t="s">
         <v>24</v>
       </c>
-      <c r="G68" s="1"/>
+      <c r="G68" s="1" t="s">
+        <v>284</v>
+      </c>
       <c r="H68" s="17">
         <v>11.258599999999999</v>
       </c>
@@ -20146,7 +20136,9 @@
       <c r="F72" t="s">
         <v>230</v>
       </c>
-      <c r="G72" s="1"/>
+      <c r="G72" s="1" t="s">
+        <v>285</v>
+      </c>
       <c r="H72" s="17">
         <v>198.25839999999999</v>
       </c>
@@ -20193,116 +20185,21 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="E75" t="s">
-        <v>232</v>
-      </c>
-      <c r="H75">
-        <v>61.9</v>
-      </c>
-      <c r="M75">
-        <v>73.099999999999994</v>
-      </c>
-      <c r="R75">
-        <v>67.2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="E76" t="s">
-        <v>233</v>
-      </c>
-      <c r="H76">
-        <v>63.9</v>
-      </c>
-      <c r="M76">
-        <v>43</v>
-      </c>
-      <c r="R76">
-        <v>67.400000000000006</v>
-      </c>
-    </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="E77" t="s">
-        <v>234</v>
-      </c>
-      <c r="H77">
-        <v>115.8</v>
-      </c>
-      <c r="M77">
-        <v>86.8</v>
-      </c>
-      <c r="R77">
-        <v>120.4</v>
-      </c>
-    </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="E78" t="s">
-        <v>236</v>
-      </c>
-      <c r="H78">
-        <v>88</v>
-      </c>
-      <c r="M78">
-        <v>63</v>
-      </c>
-      <c r="R78">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="E79" t="s">
-        <v>235</v>
-      </c>
-      <c r="H79">
-        <v>1.2E-2</v>
-      </c>
-      <c r="M79">
-        <v>0.02</v>
-      </c>
-      <c r="R79">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="E80" t="s">
-        <v>239</v>
-      </c>
-      <c r="H80" t="s">
-        <v>241</v>
-      </c>
-      <c r="M80" t="s">
-        <v>242</v>
-      </c>
-      <c r="R80" t="s">
-        <v>243</v>
-      </c>
-    </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B84" s="30" t="s">
-        <v>245</v>
-      </c>
-      <c r="C84" s="31" t="s">
-        <v>248</v>
-      </c>
+      <c r="B84" s="30"/>
+      <c r="C84" s="31"/>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B85" s="30" t="s">
-        <v>246</v>
-      </c>
-      <c r="C85" s="31" t="s">
-        <v>248</v>
-      </c>
+      <c r="B85" s="30"/>
+      <c r="C85" s="31"/>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B86" s="30" t="s">
-        <v>247</v>
-      </c>
-      <c r="C86" s="31" t="s">
-        <v>249</v>
-      </c>
+      <c r="B86" s="30"/>
+      <c r="C86" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -25695,15 +25592,15 @@
       </c>
       <c r="G75">
         <f>'1102 (not corrected)'!H75</f>
-        <v>61.9</v>
+        <v>0</v>
       </c>
       <c r="L75" s="7">
         <f>'1102 (not corrected)'!M75</f>
-        <v>73.099999999999994</v>
+        <v>0</v>
       </c>
       <c r="Q75" s="7">
         <f>'1102 (not corrected)'!R75</f>
-        <v>67.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.2">
@@ -25712,15 +25609,15 @@
       </c>
       <c r="G76">
         <f>'1102 (not corrected)'!H76</f>
-        <v>63.9</v>
+        <v>0</v>
       </c>
       <c r="L76" s="7">
         <f>'1102 (not corrected)'!M76</f>
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="Q76" s="7">
         <f>'1102 (not corrected)'!R76</f>
-        <v>67.400000000000006</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.2">
@@ -25729,15 +25626,15 @@
       </c>
       <c r="G77">
         <f>'1102 (not corrected)'!H77</f>
-        <v>115.8</v>
+        <v>0</v>
       </c>
       <c r="L77" s="7">
         <f>'1102 (not corrected)'!M77</f>
-        <v>86.8</v>
+        <v>0</v>
       </c>
       <c r="Q77" s="7">
         <f>'1102 (not corrected)'!R77</f>
-        <v>120.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.2">
@@ -25746,15 +25643,15 @@
       </c>
       <c r="G78">
         <f>'1102 (not corrected)'!H78</f>
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="L78" s="7">
         <f>'1102 (not corrected)'!M78</f>
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="Q78" s="7">
         <f>'1102 (not corrected)'!R78</f>
-        <v>92</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.2">
@@ -25763,32 +25660,32 @@
       </c>
       <c r="G79">
         <f>'1102 (not corrected)'!H79</f>
-        <v>1.2E-2</v>
+        <v>0</v>
       </c>
       <c r="L79" s="7">
         <f>'1102 (not corrected)'!M79</f>
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="Q79" s="7">
         <f>'1102 (not corrected)'!R79</f>
-        <v>0.02</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.2">
       <c r="E80" t="s">
         <v>239</v>
       </c>
-      <c r="G80" t="str">
+      <c r="G80">
         <f>'1102 (not corrected)'!H80</f>
-        <v>YL_11022023_gluc</v>
-      </c>
-      <c r="L80" s="7" t="str">
+        <v>0</v>
+      </c>
+      <c r="L80" s="7">
         <f>'1102 (not corrected)'!M80</f>
-        <v>YL_11022023_glyc</v>
-      </c>
-      <c r="Q80" s="7" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q80" s="7">
         <f>'1102 (not corrected)'!R80</f>
-        <v>YL_11022023_OA</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
worked on notebook C
</commit_message>
<xml_diff>
--- a/data/13c_mfa/INCA_model_11022023_GR.xlsx
+++ b/data/13c_mfa/INCA_model_11022023_GR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrettroell/yarrowia_eflux2/data/13c_mfa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E4CD8C-69B5-D842-83F2-60D1C66DB60F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6E2243-D3B6-3248-ACAD-9E374BEC03A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="3800" windowWidth="35840" windowHeight="18900" firstSheet="1" activeTab="3" xr2:uid="{2683B27E-BA21-2341-8B90-63D55B06C26E}"/>
+    <workbookView xWindow="280" yWindow="3800" windowWidth="27540" windowHeight="21780" firstSheet="1" activeTab="3" xr2:uid="{2683B27E-BA21-2341-8B90-63D55B06C26E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1244,9 +1244,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1284,7 +1284,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1390,7 +1390,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1532,7 +1532,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6039,7 +6039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC8C3939-0961-4E1A-B332-B7F0CF486DE2}">
   <dimension ref="A1:U80"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -15666,8 +15666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFD0AB96-9F04-41BF-A187-22CBB81F1551}">
   <dimension ref="A1:V86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G72" sqref="G72"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>